<commit_message>
Actualización tras jornada 1
</commit_message>
<xml_diff>
--- a/data/jornada_1.xlsx
+++ b/data/jornada_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,33 +456,43 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>1X2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>jornada</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>RTDO L</t>
-        </is>
-      </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>LOCAL</t>
+          <t>RTDO L.1</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>VISITANTE</t>
+          <t>LOCAL.1</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>RTDO V</t>
+          <t>VISITANTE.1</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>RTDO V.1</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>1X2.1</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -495,33 +505,39 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
+        <v>19</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>JOR. 1</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Diego</t>
-        </is>
+      <c r="G2" t="n">
+        <v>36</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
+          <t>Puche</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>Coquina</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0</v>
+      <c r="J2" t="n">
+        <v>34</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -534,33 +550,39 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="inlineStr">
+        <v>36</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>JOR. 1</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>31</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Kike</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Armada</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>0</v>
+      <c r="J3" t="n">
+        <v>49</v>
+      </c>
+      <c r="K3" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -573,28 +595,34 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="inlineStr">
+        <v>23</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>JOR. 1</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>38</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Papu</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Gonzo</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>0</v>
+      <c r="J4" t="n">
+        <v>32</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>